<commit_message>
Triggerekkel kiegeszitve es lapak felig bekotve
</commit_message>
<xml_diff>
--- a/Változók listája.xlsx
+++ b/Változók listája.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Munka\Hunify Labs\IvanVilmos_PLC_hazi_2025-01-27\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB86E9F-9753-4F59-9B6A-6C772369EFD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808E92BA-C656-493D-8735-A8976D747E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{D3870B3E-8C41-4DC9-B0DB-3C849B007305}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="73">
   <si>
     <t>Liftvezérlés változók</t>
   </si>
@@ -83,9 +83,6 @@
     <t>Szint</t>
   </si>
   <si>
-    <t>Hívógombok fel</t>
-  </si>
-  <si>
     <t>i_bGF0</t>
   </si>
   <si>
@@ -116,9 +113,6 @@
     <t>i_bGF9</t>
   </si>
   <si>
-    <t>Hívógombok le</t>
-  </si>
-  <si>
     <t>i_bGL1</t>
   </si>
   <si>
@@ -147,6 +141,120 @@
   </si>
   <si>
     <t>i_bGL10</t>
+  </si>
+  <si>
+    <t>Hívógomb lámpák LE</t>
+  </si>
+  <si>
+    <t>Hívógomb lámpák FEL</t>
+  </si>
+  <si>
+    <t>q_bLF0</t>
+  </si>
+  <si>
+    <t>q_bLF1</t>
+  </si>
+  <si>
+    <t>q_bLF2</t>
+  </si>
+  <si>
+    <t>q_bLF3</t>
+  </si>
+  <si>
+    <t>q_bLF4</t>
+  </si>
+  <si>
+    <t>q_bLF5</t>
+  </si>
+  <si>
+    <t>q_bLF6</t>
+  </si>
+  <si>
+    <t>q_bLF7</t>
+  </si>
+  <si>
+    <t>q_bLF8</t>
+  </si>
+  <si>
+    <t>q_bLF9</t>
+  </si>
+  <si>
+    <t>Hívógombok FEL</t>
+  </si>
+  <si>
+    <t>Hívógombok LE</t>
+  </si>
+  <si>
+    <t>q_bLL1</t>
+  </si>
+  <si>
+    <t>q_bLL2</t>
+  </si>
+  <si>
+    <t>q_bLL3</t>
+  </si>
+  <si>
+    <t>q_bLL4</t>
+  </si>
+  <si>
+    <t>q_bLL5</t>
+  </si>
+  <si>
+    <t>q_bLL6</t>
+  </si>
+  <si>
+    <t>q_bLL7</t>
+  </si>
+  <si>
+    <t>q_bLL8</t>
+  </si>
+  <si>
+    <t>q_bLL9</t>
+  </si>
+  <si>
+    <t>q_bLL10</t>
+  </si>
+  <si>
+    <t>Fülkegomb lámpák</t>
+  </si>
+  <si>
+    <t>q_bFGL0</t>
+  </si>
+  <si>
+    <t>q_bFGL1</t>
+  </si>
+  <si>
+    <t>q_bFGL2</t>
+  </si>
+  <si>
+    <t>q_bFGL3</t>
+  </si>
+  <si>
+    <t>q_bFGL4</t>
+  </si>
+  <si>
+    <t>q_bFGL5</t>
+  </si>
+  <si>
+    <t>q_bFGL6</t>
+  </si>
+  <si>
+    <t>q_bFGL7</t>
+  </si>
+  <si>
+    <t>q_bFGL8</t>
+  </si>
+  <si>
+    <t>q_bFGL9</t>
+  </si>
+  <si>
+    <t>q_bFGL10</t>
+  </si>
+  <si>
+    <t>BEMENET</t>
+  </si>
+  <si>
+    <t>KIEMENET</t>
   </si>
 </sst>
 </file>
@@ -196,11 +304,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -210,6 +315,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -544,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C260034B-DFDE-41FB-B549-A2E41E8A4ABF}">
-  <dimension ref="B1:I15"/>
+  <dimension ref="B1:R15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -556,276 +665,526 @@
     <col min="3" max="3" width="12.08984375" customWidth="1"/>
     <col min="6" max="6" width="11.81640625" customWidth="1"/>
     <col min="9" max="9" width="11.7265625" customWidth="1"/>
+    <col min="12" max="12" width="14.08984375" customWidth="1"/>
+    <col min="15" max="15" width="14.7265625" customWidth="1"/>
+    <col min="18" max="18" width="12.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B3" s="1" t="s">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="K2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="E3" s="1" t="s">
+      <c r="C3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="H3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="4"/>
+      <c r="K3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="4"/>
+      <c r="N3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" s="4"/>
+      <c r="Q3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="R3" s="4"/>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="H3" s="1" t="s">
+      <c r="G5" s="2"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5" t="s">
+        <v>37</v>
+      </c>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6" t="s">
+        <v>38</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2">
+        <v>2</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B5" s="2">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="K7">
         <v>2</v>
       </c>
-      <c r="E5" s="3">
-        <v>0</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B6" s="2">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="L7" t="s">
+        <v>39</v>
+      </c>
+      <c r="N7">
+        <v>2</v>
+      </c>
+      <c r="O7" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q7">
+        <v>2</v>
+      </c>
+      <c r="R7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B8" s="1">
         <v>3</v>
       </c>
-      <c r="E6" s="3">
-        <v>1</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3">
-        <v>1</v>
-      </c>
-      <c r="I6" s="3" t="s">
+      <c r="C8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="2">
+        <v>3</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2">
+        <v>3</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B7" s="2">
-        <v>2</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="K8">
+        <v>3</v>
+      </c>
+      <c r="L8" t="s">
+        <v>40</v>
+      </c>
+      <c r="N8">
+        <v>3</v>
+      </c>
+      <c r="O8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q8">
+        <v>3</v>
+      </c>
+      <c r="R8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B9" s="1">
         <v>4</v>
       </c>
-      <c r="E7" s="3">
-        <v>2</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3">
-        <v>2</v>
-      </c>
-      <c r="I7" s="3" t="s">
+      <c r="C9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="2">
+        <v>4</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2">
+        <v>4</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B8" s="2">
-        <v>3</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="K9">
+        <v>4</v>
+      </c>
+      <c r="L9" t="s">
+        <v>41</v>
+      </c>
+      <c r="N9">
+        <v>4</v>
+      </c>
+      <c r="O9" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q9">
+        <v>4</v>
+      </c>
+      <c r="R9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B10" s="1">
         <v>5</v>
       </c>
-      <c r="E8" s="3">
-        <v>3</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3">
-        <v>3</v>
-      </c>
-      <c r="I8" s="3" t="s">
+      <c r="C10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="2">
+        <v>5</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2">
+        <v>5</v>
+      </c>
+      <c r="I10" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B9" s="2">
-        <v>4</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="K10">
+        <v>5</v>
+      </c>
+      <c r="L10" t="s">
+        <v>42</v>
+      </c>
+      <c r="N10">
+        <v>5</v>
+      </c>
+      <c r="O10" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q10">
+        <v>5</v>
+      </c>
+      <c r="R10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B11" s="1">
         <v>6</v>
       </c>
-      <c r="E9" s="3">
-        <v>4</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3">
-        <v>4</v>
-      </c>
-      <c r="I9" s="3" t="s">
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="2">
+        <v>6</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2">
+        <v>6</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B10" s="2">
-        <v>5</v>
-      </c>
-      <c r="C10" s="2" t="s">
+      <c r="K11">
+        <v>6</v>
+      </c>
+      <c r="L11" t="s">
+        <v>43</v>
+      </c>
+      <c r="N11">
+        <v>6</v>
+      </c>
+      <c r="O11" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q11">
+        <v>6</v>
+      </c>
+      <c r="R11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B12" s="1">
         <v>7</v>
       </c>
-      <c r="E10" s="3">
-        <v>5</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3">
-        <v>5</v>
-      </c>
-      <c r="I10" s="3" t="s">
+      <c r="C12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="2">
+        <v>7</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2">
+        <v>7</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B11" s="2">
-        <v>6</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="K12">
+        <v>7</v>
+      </c>
+      <c r="L12" t="s">
+        <v>44</v>
+      </c>
+      <c r="N12">
+        <v>7</v>
+      </c>
+      <c r="O12" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q12">
+        <v>7</v>
+      </c>
+      <c r="R12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B13" s="1">
         <v>8</v>
       </c>
-      <c r="E11" s="3">
-        <v>6</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3">
-        <v>6</v>
-      </c>
-      <c r="I11" s="3" t="s">
+      <c r="C13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="2">
+        <v>8</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2">
+        <v>8</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B12" s="2">
-        <v>7</v>
-      </c>
-      <c r="C12" s="2" t="s">
+      <c r="K13">
+        <v>8</v>
+      </c>
+      <c r="L13" t="s">
+        <v>45</v>
+      </c>
+      <c r="N13">
+        <v>8</v>
+      </c>
+      <c r="O13" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q13">
+        <v>8</v>
+      </c>
+      <c r="R13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B14" s="1">
         <v>9</v>
       </c>
-      <c r="E12" s="3">
-        <v>7</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3">
-        <v>7</v>
-      </c>
-      <c r="I12" s="3" t="s">
+      <c r="C14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="2">
+        <v>9</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2">
+        <v>9</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B13" s="2">
-        <v>8</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="K14">
+        <v>9</v>
+      </c>
+      <c r="L14" t="s">
+        <v>46</v>
+      </c>
+      <c r="N14">
+        <v>9</v>
+      </c>
+      <c r="O14" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q14">
+        <v>9</v>
+      </c>
+      <c r="R14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B15" s="1">
         <v>10</v>
       </c>
-      <c r="E13" s="3">
-        <v>8</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3">
-        <v>8</v>
-      </c>
-      <c r="I13" s="3" t="s">
+      <c r="C15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2">
+        <v>10</v>
+      </c>
+      <c r="I15" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B14" s="2">
-        <v>9</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="3">
-        <v>9</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3">
-        <v>9</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B15" s="2">
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="N15">
         <v>10</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3">
+      <c r="O15" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q15">
         <v>10</v>
       </c>
-      <c r="I15" s="3" t="s">
-        <v>36</v>
+      <c r="R15" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="8">
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="K2:R2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="H3:I3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="N3:O3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>